<commit_message>
fix sample sizes include updated data
</commit_message>
<xml_diff>
--- a/tables/fmt/continuous-modinput.xlsx
+++ b/tables/fmt/continuous-modinput.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="136">
   <si>
     <t>Year</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>weight_zscore</t>
+  </si>
+  <si>
+    <t>treatment</t>
   </si>
   <si>
     <t>1</t>
@@ -506,10 +509,13 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
@@ -518,13 +524,13 @@
         <v>47453.0</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G2" t="n" s="2">
         <v>43250.0</v>
@@ -544,10 +550,13 @@
       <c r="L2" t="n">
         <v>-1.2126445609143655</v>
       </c>
+      <c r="M2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
@@ -556,13 +565,13 @@
         <v>47453.0</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G3" t="n" s="2">
         <v>43283.0</v>
@@ -582,10 +591,13 @@
       <c r="L3" t="n">
         <v>-0.8439640321423807</v>
       </c>
+      <c r="M3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n">
         <v>1.0</v>
@@ -594,13 +606,13 @@
         <v>47453.0</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G4" t="n" s="2">
         <v>43312.0</v>
@@ -620,10 +632,13 @@
       <c r="L4" t="n">
         <v>-0.3962805329192562</v>
       </c>
+      <c r="M4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="n">
         <v>1.0</v>
@@ -632,13 +647,13 @@
         <v>47453.0</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G5" t="n" s="2">
         <v>43343.0</v>
@@ -658,10 +673,13 @@
       <c r="L5" t="n">
         <v>0.20940890720614766</v>
       </c>
+      <c r="M5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="n">
         <v>1.0</v>
@@ -670,13 +688,13 @@
         <v>47453.0</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G6" t="n" s="2">
         <v>43374.0</v>
@@ -696,10 +714,13 @@
       <c r="L6" t="n">
         <v>0.8677669942989776</v>
       </c>
+      <c r="M6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="n">
         <v>1.0</v>
@@ -708,13 +729,13 @@
         <v>47453.0</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>43404.0</v>
@@ -734,10 +755,13 @@
       <c r="L7" t="n">
         <v>1.3944534639732415</v>
       </c>
+      <c r="M7" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="n">
         <v>1.0</v>
@@ -746,13 +770,13 @@
         <v>47453.0</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G8" t="n" s="2">
         <v>43434.0</v>
@@ -772,10 +796,13 @@
       <c r="L8" t="n">
         <v>1.7367996692615129</v>
       </c>
+      <c r="M8" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="n">
         <v>1.0</v>
@@ -784,13 +811,13 @@
         <v>47455.0</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G9" t="n" s="2">
         <v>43251.0</v>
@@ -810,10 +837,13 @@
       <c r="L9" t="n">
         <v>-1.423319148784071</v>
       </c>
+      <c r="M9" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="n">
         <v>1.0</v>
@@ -822,13 +852,13 @@
         <v>47455.0</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G10" t="n" s="2">
         <v>43283.0</v>
@@ -848,10 +878,13 @@
       <c r="L10" t="n">
         <v>-1.0546386200120863</v>
       </c>
+      <c r="M10" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="n">
         <v>1.0</v>
@@ -860,13 +893,13 @@
         <v>47455.0</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G11" t="n" s="2">
         <v>43312.0</v>
@@ -886,10 +919,13 @@
       <c r="L11" t="n">
         <v>-0.7912953851749542</v>
       </c>
+      <c r="M11" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" t="n">
         <v>1.0</v>
@@ -898,13 +934,13 @@
         <v>47455.0</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G12" t="n" s="2">
         <v>43343.0</v>
@@ -924,10 +960,13 @@
       <c r="L12" t="n">
         <v>-0.3962805329192562</v>
       </c>
+      <c r="M12" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="n">
         <v>1.0</v>
@@ -936,13 +975,13 @@
         <v>47455.0</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G13" t="n" s="2">
         <v>43374.0</v>
@@ -962,10 +1001,13 @@
       <c r="L13" t="n">
         <v>0.025068642820155095</v>
       </c>
+      <c r="M13" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" t="n">
         <v>1.0</v>
@@ -974,13 +1016,13 @@
         <v>47455.0</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G14" t="n" s="2">
         <v>43404.0</v>
@@ -1000,10 +1042,13 @@
       <c r="L14" t="n">
         <v>0.3410805246247132</v>
       </c>
+      <c r="M14" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="n">
         <v>1.0</v>
@@ -1012,13 +1057,13 @@
         <v>47455.0</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G15" t="n" s="2">
         <v>43434.0</v>
@@ -1038,10 +1083,13 @@
       <c r="L15" t="n">
         <v>0.3410805246247132</v>
       </c>
+      <c r="M15" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="n">
         <v>1.0</v>
@@ -1050,13 +1098,13 @@
         <v>47457.0</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G16" t="n" s="2">
         <v>43252.0</v>
@@ -1076,10 +1124,13 @@
       <c r="L16" t="n">
         <v>-1.2653132078817917</v>
       </c>
+      <c r="M16" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="n">
         <v>1.0</v>
@@ -1088,13 +1139,13 @@
         <v>47457.0</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G17" t="n" s="2">
         <v>43283.0</v>
@@ -1114,10 +1165,13 @@
       <c r="L17" t="n">
         <v>-0.9493013260772333</v>
       </c>
+      <c r="M17" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
@@ -1126,13 +1180,13 @@
         <v>47457.0</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G18" t="n" s="2">
         <v>43312.0</v>
@@ -1152,10 +1206,13 @@
       <c r="L18" t="n">
         <v>-0.4752835033703959</v>
       </c>
+      <c r="M18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="n">
         <v>1.0</v>
@@ -1164,13 +1221,13 @@
         <v>47457.0</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G19" t="n" s="2">
         <v>43343.0</v>
@@ -1190,10 +1247,13 @@
       <c r="L19" t="n">
         <v>0.05140296630386832</v>
       </c>
+      <c r="M19" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="n">
         <v>1.0</v>
@@ -1202,13 +1262,13 @@
         <v>47457.0</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G20" t="n" s="2">
         <v>43374.0</v>
@@ -1228,10 +1288,13 @@
       <c r="L20" t="n">
         <v>0.5254207890107058</v>
       </c>
+      <c r="M20" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="n">
         <v>1.0</v>
@@ -1240,13 +1303,13 @@
         <v>47457.0</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G21" t="n" s="2">
         <v>43404.0</v>
@@ -1266,10 +1329,13 @@
       <c r="L21" t="n">
         <v>0.8677669942989776</v>
       </c>
+      <c r="M21" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="n">
         <v>1.0</v>
@@ -1278,13 +1344,13 @@
         <v>47457.0</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G22" t="n" s="2">
         <v>43434.0</v>
@@ -1304,10 +1370,13 @@
       <c r="L22" t="n">
         <v>1.1837788761035357</v>
       </c>
+      <c r="M22" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="n">
         <v>1.0</v>
@@ -1316,13 +1385,13 @@
         <v>47467.0</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G23" t="n" s="2">
         <v>43255.0</v>
@@ -1342,10 +1411,13 @@
       <c r="L23" t="n">
         <v>-1.5023221192352108</v>
       </c>
+      <c r="M23" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" t="n">
         <v>1.0</v>
@@ -1354,13 +1426,13 @@
         <v>47467.0</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G24" t="n" s="2">
         <v>43265.0</v>
@@ -1380,10 +1452,13 @@
       <c r="L24" t="n">
         <v>-1.3969848253003578</v>
       </c>
+      <c r="M24" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="n">
         <v>1.0</v>
@@ -1392,13 +1467,13 @@
         <v>47467.0</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G25" t="n" s="2">
         <v>43272.0</v>
@@ -1418,10 +1493,13 @@
       <c r="L25" t="n">
         <v>-1.3179818548492181</v>
       </c>
+      <c r="M25" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" t="n">
         <v>1.0</v>
@@ -1430,13 +1508,13 @@
         <v>47467.0</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G26" t="n" s="2">
         <v>43287.0</v>
@@ -1456,10 +1534,13 @@
       <c r="L26" t="n">
         <v>-1.1073072669795128</v>
       </c>
+      <c r="M26" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" t="n">
         <v>1.0</v>
@@ -1468,13 +1549,13 @@
         <v>47467.0</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G27" t="n" s="2">
         <v>43318.0</v>
@@ -1494,10 +1575,13 @@
       <c r="L27" t="n">
         <v>-0.764961061691241</v>
       </c>
+      <c r="M27" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="n">
         <v>1.0</v>
@@ -1506,13 +1590,13 @@
         <v>47467.0</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G28" t="n" s="2">
         <v>43347.0</v>
@@ -1532,10 +1616,13 @@
       <c r="L28" t="n">
         <v>-0.3172775624681165</v>
       </c>
+      <c r="M28" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" t="n">
         <v>1.0</v>
@@ -1544,13 +1631,13 @@
         <v>47467.0</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G29" t="n" s="2">
         <v>43409.0</v>
@@ -1570,10 +1657,13 @@
       <c r="L29" t="n">
         <v>0.5254207890107058</v>
       </c>
+      <c r="M29" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B30" t="n">
         <v>1.0</v>
@@ -1582,13 +1672,13 @@
         <v>47467.0</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G30" t="n" s="2">
         <v>43439.0</v>
@@ -1608,10 +1698,13 @@
       <c r="L30" t="n">
         <v>0.6307580829455587</v>
       </c>
+      <c r="M30" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
         <v>1.0</v>
@@ -1620,13 +1713,13 @@
         <v>47470.0</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G31" t="n" s="2">
         <v>43256.0</v>
@@ -1646,10 +1739,13 @@
       <c r="L31" t="n">
         <v>-1.1599759139469392</v>
       </c>
+      <c r="M31" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" t="n">
         <v>1.0</v>
@@ -1658,13 +1754,13 @@
         <v>47470.0</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G32" t="n" s="2">
         <v>43287.0</v>
@@ -1684,10 +1780,13 @@
       <c r="L32" t="n">
         <v>-0.9229670025935204</v>
       </c>
+      <c r="M32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B33" t="n">
         <v>1.0</v>
@@ -1696,13 +1795,13 @@
         <v>47470.0</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G33" t="n" s="2">
         <v>43318.0</v>
@@ -1722,10 +1821,13 @@
       <c r="L33" t="n">
         <v>-0.501617826854109</v>
       </c>
+      <c r="M33" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" t="n">
         <v>1.0</v>
@@ -1734,13 +1836,13 @@
         <v>47470.0</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E34" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G34" t="n" s="2">
         <v>43347.0</v>
@@ -1760,10 +1862,13 @@
       <c r="L34" t="n">
         <v>-0.053934327630984574</v>
       </c>
+      <c r="M34" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" t="n">
         <v>1.0</v>
@@ -1772,13 +1877,13 @@
         <v>47470.0</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G35" t="n" s="2">
         <v>43409.0</v>
@@ -1798,10 +1903,13 @@
       <c r="L35" t="n">
         <v>0.6834267299129851</v>
       </c>
+      <c r="M35" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" t="n">
         <v>1.0</v>
@@ -1810,13 +1918,13 @@
         <v>47470.0</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G36" t="n" s="2">
         <v>43439.0</v>
@@ -1836,10 +1944,13 @@
       <c r="L36" t="n">
         <v>0.8941013177826903</v>
       </c>
+      <c r="M36" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B37" t="n">
         <v>1.0</v>
@@ -1848,13 +1959,13 @@
         <v>47487.0</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G37" t="n" s="2">
         <v>43262.0</v>
@@ -1874,10 +1985,13 @@
       <c r="L37" t="n">
         <v>-1.0019699730446598</v>
       </c>
+      <c r="M37" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" t="n">
         <v>1.0</v>
@@ -1886,13 +2000,13 @@
         <v>47487.0</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E38" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G38" t="n" s="2">
         <v>43292.0</v>
@@ -1912,10 +2026,13 @@
       <c r="L38" t="n">
         <v>-0.764961061691241</v>
       </c>
+      <c r="M38" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" t="n">
         <v>1.0</v>
@@ -1924,13 +2041,13 @@
         <v>47487.0</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G39" t="n" s="2">
         <v>43325.0</v>
@@ -1950,10 +2067,13 @@
       <c r="L39" t="n">
         <v>-0.2646089155006904</v>
       </c>
+      <c r="M39" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" t="n">
         <v>1.0</v>
@@ -1962,13 +2082,13 @@
         <v>47487.0</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G40" t="n" s="2">
         <v>43354.0</v>
@@ -1988,10 +2108,13 @@
       <c r="L40" t="n">
         <v>0.18307458372243443</v>
       </c>
+      <c r="M40" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" t="n">
         <v>1.0</v>
@@ -2000,13 +2123,13 @@
         <v>47487.0</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G41" t="n" s="2">
         <v>43384.0</v>
@@ -2026,10 +2149,13 @@
       <c r="L41" t="n">
         <v>0.6570924064292719</v>
       </c>
+      <c r="M41" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" t="n">
         <v>1.0</v>
@@ -2038,13 +2164,13 @@
         <v>47487.0</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" t="n" s="2">
         <v>43409.0</v>
@@ -2064,10 +2190,13 @@
       <c r="L42" t="n">
         <v>0.9467699647501168</v>
       </c>
+      <c r="M42" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" t="n">
         <v>1.0</v>
@@ -2076,13 +2205,13 @@
         <v>47487.0</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G43" t="n" s="2">
         <v>43439.0</v>
@@ -2102,10 +2231,13 @@
       <c r="L43" t="n">
         <v>0.9204356412664035</v>
       </c>
+      <c r="M43" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44" t="n">
         <v>1.0</v>
@@ -2114,13 +2246,13 @@
         <v>47557.0</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G44" t="n" s="2">
         <v>43298.0</v>
@@ -2140,10 +2272,13 @@
       <c r="L44" t="n">
         <v>-1.6076594131700637</v>
       </c>
+      <c r="M44" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" t="n">
         <v>1.0</v>
@@ -2152,13 +2287,13 @@
         <v>47557.0</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G45" t="n" s="2">
         <v>43328.0</v>
@@ -2178,10 +2313,13 @@
       <c r="L45" t="n">
         <v>-1.3969848253003578</v>
       </c>
+      <c r="M45" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46" t="n">
         <v>1.0</v>
@@ -2190,13 +2328,13 @@
         <v>47557.0</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G46" t="n" s="2">
         <v>43360.0</v>
@@ -2216,10 +2354,13 @@
       <c r="L46" t="n">
         <v>-0.9493013260772333</v>
       </c>
+      <c r="M46" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" t="n">
         <v>1.0</v>
@@ -2228,13 +2369,13 @@
         <v>47557.0</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E47" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G47" t="n" s="2">
         <v>43419.0</v>
@@ -2254,10 +2395,13 @@
       <c r="L47" t="n">
         <v>0.05140296630386832</v>
       </c>
+      <c r="M47" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48" t="n">
         <v>1.0</v>
@@ -2266,13 +2410,13 @@
         <v>47557.0</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G48" t="n" s="2">
         <v>43451.0</v>
@@ -2292,10 +2436,13 @@
       <c r="L48" t="n">
         <v>0.6307580829455587</v>
       </c>
+      <c r="M48" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49" t="n">
         <v>1.0</v>
@@ -2304,13 +2451,13 @@
         <v>47557.0</v>
       </c>
       <c r="D49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E49" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G49" t="n" s="2">
         <v>43481.0</v>
@@ -2330,10 +2477,13 @@
       <c r="L49" t="n">
         <v>0.7887640238478381</v>
       </c>
+      <c r="M49" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50" t="n">
         <v>2.0</v>
@@ -2342,13 +2492,13 @@
         <v>48429.0</v>
       </c>
       <c r="D50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F50" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G50" t="n" s="2">
         <v>43728.0</v>
@@ -2368,10 +2518,13 @@
       <c r="L50" t="n">
         <v>-1.3969848253003578</v>
       </c>
+      <c r="M50" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" t="n">
         <v>2.0</v>
@@ -2380,13 +2533,13 @@
         <v>48429.0</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E51" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G51" t="n" s="2">
         <v>43759.0</v>
@@ -2406,10 +2559,13 @@
       <c r="L51" t="n">
         <v>-1.028304296528373</v>
       </c>
+      <c r="M51" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52" t="n">
         <v>2.0</v>
@@ -2418,13 +2574,13 @@
         <v>48429.0</v>
       </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G52" t="n" s="2">
         <v>43788.0</v>
@@ -2444,10 +2600,13 @@
       <c r="L52" t="n">
         <v>-0.6859580912401013</v>
       </c>
+      <c r="M52" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" t="n">
         <v>2.0</v>
@@ -2456,13 +2615,13 @@
         <v>48429.0</v>
       </c>
       <c r="D53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E53" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G53" t="n" s="2">
         <v>43816.0</v>
@@ -2482,10 +2641,13 @@
       <c r="L53" t="n">
         <v>-0.34361188595182973</v>
       </c>
+      <c r="M53" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" t="n">
         <v>2.0</v>
@@ -2494,13 +2656,13 @@
         <v>48429.0</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E54" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G54" t="n" s="2">
         <v>43846.0</v>
@@ -2520,10 +2682,13 @@
       <c r="L54" t="n">
         <v>0.05140296630386832</v>
       </c>
+      <c r="M54" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B55" t="n">
         <v>2.0</v>
@@ -2532,13 +2697,13 @@
         <v>48429.0</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E55" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F55" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G55" t="n" s="2">
         <v>43881.0</v>
@@ -2558,10 +2723,13 @@
       <c r="L55" t="n">
         <v>0.6834267299129851</v>
       </c>
+      <c r="M55" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B56" t="n">
         <v>2.0</v>
@@ -2570,13 +2738,13 @@
         <v>48429.0</v>
       </c>
       <c r="D56" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E56" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G56" t="n" s="2">
         <v>43910.0</v>
@@ -2596,10 +2764,13 @@
       <c r="L56" t="n">
         <v>1.3154504935221019</v>
       </c>
+      <c r="M56" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57" t="n">
         <v>3.0</v>
@@ -2608,13 +2779,13 @@
         <v>50674.0</v>
       </c>
       <c r="D57" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E57" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F57" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G57" t="n" s="2">
         <v>44712.0</v>
@@ -2634,10 +2805,13 @@
       <c r="L57" t="n">
         <v>-1.2389788843980787</v>
       </c>
+      <c r="M57" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B58" t="n">
         <v>3.0</v>
@@ -2646,13 +2820,13 @@
         <v>50674.0</v>
       </c>
       <c r="D58" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E58" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G58" t="n" s="2">
         <v>44742.0</v>
@@ -2672,10 +2846,13 @@
       <c r="L58" t="n">
         <v>-1.0019699730446598</v>
       </c>
+      <c r="M58" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59" t="n">
         <v>3.0</v>
@@ -2684,13 +2861,13 @@
         <v>50674.0</v>
       </c>
       <c r="D59" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E59" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G59" t="n" s="2">
         <v>44774.0</v>
@@ -2710,10 +2887,13 @@
       <c r="L59" t="n">
         <v>-0.8439640321423807</v>
       </c>
+      <c r="M59" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60" t="n">
         <v>3.0</v>
@@ -2722,13 +2902,13 @@
         <v>50674.0</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E60" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F60" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G60" t="n" s="2">
         <v>44804.0</v>
@@ -2748,10 +2928,13 @@
       <c r="L60" t="n">
         <v>-0.6069551207889617</v>
       </c>
+      <c r="M60" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B61" t="n">
         <v>3.0</v>
@@ -2760,13 +2943,13 @@
         <v>50674.0</v>
       </c>
       <c r="D61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E61" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F61" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G61" t="n" s="2">
         <v>44834.0</v>
@@ -2786,10 +2969,13 @@
       <c r="L61" t="n">
         <v>-0.15927162156583746</v>
       </c>
+      <c r="M61" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B62" t="n">
         <v>3.0</v>
@@ -2798,13 +2984,13 @@
         <v>50674.0</v>
       </c>
       <c r="D62" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E62" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G62" t="n" s="2">
         <v>44865.0</v>
@@ -2824,10 +3010,13 @@
       <c r="L62" t="n">
         <v>0.3410805246247132</v>
       </c>
+      <c r="M62" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B63" t="n">
         <v>3.0</v>
@@ -2836,13 +3025,13 @@
         <v>50674.0</v>
       </c>
       <c r="D63" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E63" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G63" t="n" s="2">
         <v>44872.0</v>
@@ -2862,10 +3051,13 @@
       <c r="L63" t="n">
         <v>0.49908646552699254</v>
       </c>
+      <c r="M63" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B64" t="n">
         <v>3.0</v>
@@ -2874,13 +3066,13 @@
         <v>50674.0</v>
       </c>
       <c r="D64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E64" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F64" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G64" t="n" s="2">
         <v>44888.0</v>
@@ -2900,10 +3092,13 @@
       <c r="L64" t="n">
         <v>1.0257729352012563</v>
       </c>
+      <c r="M64" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B65" t="n">
         <v>3.0</v>
@@ -2912,13 +3107,13 @@
         <v>50674.0</v>
       </c>
       <c r="D65" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E65" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F65" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G65" t="n" s="2">
         <v>44902.0</v>
@@ -2938,10 +3133,13 @@
       <c r="L65" t="n">
         <v>0.7624297003641248</v>
       </c>
+      <c r="M65" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B66" t="n">
         <v>3.0</v>
@@ -2950,13 +3148,13 @@
         <v>50691.0</v>
       </c>
       <c r="D66" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E66" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G66" t="n" s="2">
         <v>44719.0</v>
@@ -2976,10 +3174,13 @@
       <c r="L66" t="n">
         <v>-1.3179818548492181</v>
       </c>
+      <c r="M66" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B67" t="n">
         <v>3.0</v>
@@ -2988,13 +3189,13 @@
         <v>50691.0</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E67" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F67" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G67" t="n" s="2">
         <v>44725.0</v>
@@ -3014,10 +3215,13 @@
       <c r="L67" t="n">
         <v>-1.1863102374306524</v>
       </c>
+      <c r="M67" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B68" t="n">
         <v>3.0</v>
@@ -3026,13 +3230,13 @@
         <v>50691.0</v>
       </c>
       <c r="D68" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E68" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F68" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G68" t="n" s="2">
         <v>44750.0</v>
@@ -3052,10 +3256,13 @@
       <c r="L68" t="n">
         <v>-0.8439640321423807</v>
       </c>
+      <c r="M68" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B69" t="n">
         <v>3.0</v>
@@ -3064,13 +3271,13 @@
         <v>50691.0</v>
       </c>
       <c r="D69" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E69" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G69" t="n" s="2">
         <v>44782.0</v>
@@ -3090,10 +3297,13 @@
       <c r="L69" t="n">
         <v>-0.3172775624681165</v>
       </c>
+      <c r="M69" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70" t="n">
         <v>3.0</v>
@@ -3102,13 +3312,13 @@
         <v>50691.0</v>
       </c>
       <c r="D70" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E70" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F70" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G70" t="n" s="2">
         <v>44813.0</v>
@@ -3128,10 +3338,13 @@
       <c r="L70" t="n">
         <v>0.15674026023872123</v>
       </c>
+      <c r="M70" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" t="n">
         <v>3.0</v>
@@ -3140,13 +3353,13 @@
         <v>50691.0</v>
       </c>
       <c r="D71" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F71" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G71" t="n" s="2">
         <v>44841.0</v>
@@ -3166,10 +3379,13 @@
       <c r="L71" t="n">
         <v>0.42008349507585285</v>
       </c>
+      <c r="M71" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72" t="n">
         <v>3.0</v>
@@ -3178,13 +3394,13 @@
         <v>50691.0</v>
       </c>
       <c r="D72" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E72" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G72" t="n" s="2">
         <v>44872.0</v>
@@ -3204,10 +3420,13 @@
       <c r="L72" t="n">
         <v>-0.15927162156583746</v>
       </c>
+      <c r="M72" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B73" t="n">
         <v>3.0</v>
@@ -3216,13 +3435,13 @@
         <v>50691.0</v>
       </c>
       <c r="D73" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F73" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G73" t="n" s="2">
         <v>44873.0</v>
@@ -3242,10 +3461,13 @@
       <c r="L73" t="n">
         <v>0.15674026023872123</v>
       </c>
+      <c r="M73" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74" t="n">
         <v>3.0</v>
@@ -3254,13 +3476,13 @@
         <v>50691.0</v>
       </c>
       <c r="D74" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E74" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F74" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G74" t="n" s="2">
         <v>44876.0</v>
@@ -3280,10 +3502,13 @@
       <c r="L74" t="n">
         <v>-0.269875780197433</v>
       </c>
+      <c r="M74" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B75" t="n">
         <v>3.0</v>
@@ -3292,13 +3517,13 @@
         <v>50691.0</v>
       </c>
       <c r="D75" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F75" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G75" t="n" s="2">
         <v>44877.0</v>
@@ -3318,10 +3543,13 @@
       <c r="L75" t="n">
         <v>-0.2435414567137198</v>
       </c>
+      <c r="M75" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B76" t="n">
         <v>3.0</v>
@@ -3330,13 +3558,13 @@
         <v>50691.0</v>
       </c>
       <c r="D76" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E76" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F76" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G76" t="n" s="2">
         <v>44879.0</v>
@@ -3356,10 +3584,13 @@
       <c r="L76" t="e">
         <v>#N/A</v>
       </c>
+      <c r="M76" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B77" t="n">
         <v>3.0</v>
@@ -3368,13 +3599,13 @@
         <v>50691.0</v>
       </c>
       <c r="D77" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E77" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F77" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G77" t="n" s="2">
         <v>44882.0</v>
@@ -3394,10 +3625,13 @@
       <c r="L77" t="n">
         <v>-0.16980535095932275</v>
       </c>
+      <c r="M77" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B78" t="n">
         <v>3.0</v>
@@ -3406,13 +3640,13 @@
         <v>50731.0</v>
       </c>
       <c r="D78" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E78" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F78" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G78" t="n" s="2">
         <v>44736.0</v>
@@ -3432,10 +3666,13 @@
       <c r="L78" t="n">
         <v>-1.1073072669795128</v>
       </c>
+      <c r="M78" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B79" t="n">
         <v>3.0</v>
@@ -3444,13 +3681,13 @@
         <v>50731.0</v>
       </c>
       <c r="D79" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E79" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F79" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G79" t="n" s="2">
         <v>44742.0</v>
@@ -3470,10 +3707,13 @@
       <c r="L79" t="n">
         <v>-1.0546386200120863</v>
       </c>
+      <c r="M79" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B80" t="n">
         <v>3.0</v>
@@ -3482,13 +3722,13 @@
         <v>50731.0</v>
       </c>
       <c r="D80" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E80" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F80" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G80" t="n" s="2">
         <v>44743.0</v>
@@ -3508,10 +3748,13 @@
       <c r="L80" t="n">
         <v>-1.0546386200120863</v>
       </c>
+      <c r="M80" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B81" t="n">
         <v>3.0</v>
@@ -3520,13 +3763,13 @@
         <v>50731.0</v>
       </c>
       <c r="D81" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E81" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F81" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G81" t="n" s="2">
         <v>44764.0</v>
@@ -3546,10 +3789,13 @@
       <c r="L81" t="n">
         <v>-0.764961061691241</v>
       </c>
+      <c r="M81" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B82" t="n">
         <v>3.0</v>
@@ -3558,13 +3804,13 @@
         <v>50731.0</v>
       </c>
       <c r="D82" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E82" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F82" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G82" t="n" s="2">
         <v>44795.0</v>
@@ -3584,10 +3830,13 @@
       <c r="L82" t="n">
         <v>-0.2646089155006904</v>
       </c>
+      <c r="M82" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83" t="n">
         <v>3.0</v>
@@ -3596,13 +3845,13 @@
         <v>50731.0</v>
       </c>
       <c r="D83" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E83" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F83" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G83" t="n" s="2">
         <v>44826.0</v>
@@ -3622,10 +3871,13 @@
       <c r="L83" t="n">
         <v>0.130405936755008</v>
       </c>
+      <c r="M83" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B84" t="n">
         <v>3.0</v>
@@ -3634,13 +3886,13 @@
         <v>50731.0</v>
       </c>
       <c r="D84" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E84" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F84" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G84" t="n" s="2">
         <v>44828.0</v>
@@ -3660,10 +3912,13 @@
       <c r="L84" t="n">
         <v>0.20940890720614766</v>
       </c>
+      <c r="M84" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85" t="n">
         <v>3.0</v>
@@ -3672,13 +3927,13 @@
         <v>50731.0</v>
       </c>
       <c r="D85" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E85" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F85" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G85" t="n" s="2">
         <v>44855.0</v>
@@ -3698,10 +3953,13 @@
       <c r="L85" t="n">
         <v>0.7097610533966984</v>
       </c>
+      <c r="M85" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B86" t="n">
         <v>3.0</v>
@@ -3710,13 +3968,13 @@
         <v>50731.0</v>
       </c>
       <c r="D86" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E86" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F86" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G86" t="n" s="2">
         <v>44887.0</v>
@@ -3736,10 +3994,13 @@
       <c r="L86" t="n">
         <v>1.1574445526198225</v>
       </c>
+      <c r="M86" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B87" t="n">
         <v>3.0</v>
@@ -3748,13 +4009,13 @@
         <v>50731.0</v>
       </c>
       <c r="D87" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E87" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F87" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G87" t="n" s="2">
         <v>44895.0</v>
@@ -3774,10 +4035,13 @@
       <c r="L87" t="n">
         <v>1.210113199587249</v>
       </c>
+      <c r="M87" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" t="n">
         <v>3.0</v>
@@ -3786,13 +4050,13 @@
         <v>50731.0</v>
       </c>
       <c r="D88" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E88" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F88" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G88" t="n" s="2">
         <v>44902.0</v>
@@ -3812,10 +4076,13 @@
       <c r="L88" t="n">
         <v>1.2627818465546754</v>
       </c>
+      <c r="M88" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B89" t="n">
         <v>3.0</v>
@@ -3824,13 +4091,13 @@
         <v>50731.0</v>
       </c>
       <c r="D89" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E89" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F89" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G89" t="n" s="2">
         <v>44924.0</v>
@@ -3850,10 +4117,13 @@
       <c r="L89" t="n">
         <v>1.4997907579080945</v>
       </c>
+      <c r="M89" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B90" t="n">
         <v>3.0</v>
@@ -3862,13 +4132,13 @@
         <v>50740.0</v>
       </c>
       <c r="D90" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E90" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F90" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G90" t="n" s="2">
         <v>44742.0</v>
@@ -3888,10 +4158,13 @@
       <c r="L90" t="n">
         <v>-1.275846937275277</v>
       </c>
+      <c r="M90" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B91" t="n">
         <v>3.0</v>
@@ -3900,13 +4173,13 @@
         <v>50740.0</v>
       </c>
       <c r="D91" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E91" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F91" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G91" t="n" s="2">
         <v>44748.0</v>
@@ -3926,10 +4199,13 @@
       <c r="L91" t="n">
         <v>-1.1863102374306524</v>
       </c>
+      <c r="M91" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B92" t="n">
         <v>3.0</v>
@@ -3938,13 +4214,13 @@
         <v>50740.0</v>
       </c>
       <c r="D92" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E92" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F92" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G92" t="n" s="2">
         <v>44749.0</v>
@@ -3964,10 +4240,13 @@
       <c r="L92" t="n">
         <v>-1.1863102374306524</v>
       </c>
+      <c r="M92" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B93" t="n">
         <v>3.0</v>
@@ -3976,13 +4255,13 @@
         <v>50740.0</v>
       </c>
       <c r="D93" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E93" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F93" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G93" t="n" s="2">
         <v>44774.0</v>
@@ -4002,10 +4281,13 @@
       <c r="L93" t="n">
         <v>-0.8439640321423807</v>
       </c>
+      <c r="M93" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B94" t="n">
         <v>3.0</v>
@@ -4014,13 +4296,13 @@
         <v>50740.0</v>
       </c>
       <c r="D94" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E94" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F94" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G94" t="n" s="2">
         <v>44804.0</v>
@@ -4040,10 +4322,13 @@
       <c r="L94" t="n">
         <v>-0.36994620943554296</v>
       </c>
+      <c r="M94" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95" t="n">
         <v>3.0</v>
@@ -4052,13 +4337,13 @@
         <v>50740.0</v>
       </c>
       <c r="D95" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E95" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F95" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G95" t="n" s="2">
         <v>44834.0</v>
@@ -4078,10 +4363,13 @@
       <c r="L95" t="n">
         <v>-0.053934327630984574</v>
       </c>
+      <c r="M95" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96" t="n">
         <v>3.0</v>
@@ -4090,13 +4378,13 @@
         <v>50740.0</v>
       </c>
       <c r="D96" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E96" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F96" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G96" t="n" s="2">
         <v>44865.0</v>
@@ -4116,10 +4404,13 @@
       <c r="L96" t="n">
         <v>0.3410805246247132</v>
       </c>
+      <c r="M96" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B97" t="n">
         <v>3.0</v>
@@ -4128,13 +4419,13 @@
         <v>50740.0</v>
       </c>
       <c r="D97" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E97" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F97" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G97" t="n" s="2">
         <v>44895.0</v>
@@ -4154,10 +4445,13 @@
       <c r="L97" t="n">
         <v>0.6834267299129851</v>
       </c>
+      <c r="M97" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B98" t="n">
         <v>3.0</v>
@@ -4166,13 +4460,13 @@
         <v>50740.0</v>
       </c>
       <c r="D98" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E98" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F98" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G98" t="n" s="2">
         <v>44902.0</v>
@@ -4192,10 +4486,13 @@
       <c r="L98" t="n">
         <v>0.7887640238478381</v>
       </c>
+      <c r="M98" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B99" t="n">
         <v>3.0</v>
@@ -4204,13 +4501,13 @@
         <v>50740.0</v>
       </c>
       <c r="D99" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E99" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F99" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G99" t="n" s="2">
         <v>44924.0</v>
@@ -4230,10 +4527,13 @@
       <c r="L99" t="n">
         <v>1.104775905652396</v>
       </c>
+      <c r="M99" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B100" t="n">
         <v>3.0</v>
@@ -4242,13 +4542,13 @@
         <v>50752.0</v>
       </c>
       <c r="D100" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E100" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F100" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G100" t="n" s="2">
         <v>44747.0</v>
@@ -4268,10 +4568,13 @@
       <c r="L100" t="n">
         <v>-1.4759877957514975</v>
       </c>
+      <c r="M100" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B101" t="n">
         <v>3.0</v>
@@ -4280,13 +4583,13 @@
         <v>50752.0</v>
       </c>
       <c r="D101" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E101" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F101" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G101" t="n" s="2">
         <v>44753.0</v>
@@ -4306,10 +4609,13 @@
       <c r="L101" t="n">
         <v>-1.423319148784071</v>
       </c>
+      <c r="M101" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B102" t="n">
         <v>3.0</v>
@@ -4318,13 +4624,13 @@
         <v>50752.0</v>
       </c>
       <c r="D102" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E102" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F102" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G102" t="n" s="2">
         <v>44755.0</v>
@@ -4344,10 +4650,13 @@
       <c r="L102" t="n">
         <v>-1.4496534722677843</v>
       </c>
+      <c r="M102" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B103" t="n">
         <v>3.0</v>
@@ -4356,13 +4665,13 @@
         <v>50752.0</v>
       </c>
       <c r="D103" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E103" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F103" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G103" t="n" s="2">
         <v>44778.0</v>
@@ -4382,10 +4691,13 @@
       <c r="L103" t="n">
         <v>-1.2389788843980787</v>
       </c>
+      <c r="M103" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104" t="n">
         <v>3.0</v>
@@ -4394,13 +4706,13 @@
         <v>50752.0</v>
       </c>
       <c r="D104" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E104" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F104" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G104" t="n" s="2">
         <v>44810.0</v>
@@ -4420,10 +4732,13 @@
       <c r="L104" t="n">
         <v>-0.7386267382075278</v>
       </c>
+      <c r="M104" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B105" t="n">
         <v>3.0</v>
@@ -4432,13 +4747,13 @@
         <v>50752.0</v>
       </c>
       <c r="D105" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E105" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F105" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G105" t="n" s="2">
         <v>44840.0</v>
@@ -4458,10 +4773,13 @@
       <c r="L105" t="n">
         <v>-0.1856059450495507</v>
       </c>
+      <c r="M105" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B106" t="n">
         <v>3.0</v>
@@ -4470,13 +4788,13 @@
         <v>50752.0</v>
       </c>
       <c r="D106" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E106" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F106" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G106" t="n" s="2">
         <v>44841.0</v>
@@ -4496,10 +4814,13 @@
       <c r="L106" t="n">
         <v>-0.1856059450495507</v>
       </c>
+      <c r="M106" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B107" t="n">
         <v>3.0</v>
@@ -4508,13 +4829,13 @@
         <v>50752.0</v>
       </c>
       <c r="D107" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E107" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F107" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G107" t="n" s="2">
         <v>44872.0</v>
@@ -4534,10 +4855,13 @@
       <c r="L107" t="n">
         <v>0.2357432306898603</v>
       </c>
+      <c r="M107" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B108" t="n">
         <v>3.0</v>
@@ -4546,13 +4870,13 @@
         <v>50752.0</v>
       </c>
       <c r="D108" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E108" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F108" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G108" t="n" s="2">
         <v>44900.0</v>
@@ -4572,10 +4896,13 @@
       <c r="L108" t="n">
         <v>0.6834267299129851</v>
       </c>
+      <c r="M108" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B109" t="n">
         <v>3.0</v>
@@ -4584,13 +4911,13 @@
         <v>50752.0</v>
       </c>
       <c r="D109" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E109" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F109" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G109" t="n" s="2">
         <v>44908.0</v>
@@ -4610,10 +4937,13 @@
       <c r="L109" t="n">
         <v>0.8941013177826903</v>
       </c>
+      <c r="M109" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B110" t="n">
         <v>3.0</v>
@@ -4622,13 +4952,13 @@
         <v>50752.0</v>
       </c>
       <c r="D110" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E110" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F110" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G110" t="n" s="2">
         <v>44938.0</v>
@@ -4648,10 +4978,13 @@
       <c r="L110" t="n">
         <v>1.1574445526198225</v>
       </c>
+      <c r="M110" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B111" t="n">
         <v>3.0</v>
@@ -4660,13 +4993,13 @@
         <v>50776.0</v>
       </c>
       <c r="D111" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E111" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F111" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G111" t="n" s="2">
         <v>44763.0</v>
@@ -4686,10 +5019,13 @@
       <c r="L111" t="n">
         <v>-1.3706505018166446</v>
       </c>
+      <c r="M111" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B112" t="n">
         <v>3.0</v>
@@ -4698,13 +5034,13 @@
         <v>50776.0</v>
       </c>
       <c r="D112" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E112" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F112" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G112" t="n" s="2">
         <v>44769.0</v>
@@ -4724,10 +5060,13 @@
       <c r="L112" t="n">
         <v>-1.3443161783329314</v>
       </c>
+      <c r="M112" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B113" t="n">
         <v>3.0</v>
@@ -4736,13 +5075,13 @@
         <v>50776.0</v>
       </c>
       <c r="D113" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E113" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F113" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G113" t="n" s="2">
         <v>44771.0</v>
@@ -4762,10 +5101,13 @@
       <c r="L113" t="n">
         <v>-1.3179818548492181</v>
       </c>
+      <c r="M113" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B114" t="n">
         <v>3.0</v>
@@ -4774,13 +5116,13 @@
         <v>50776.0</v>
       </c>
       <c r="D114" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E114" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F114" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G114" t="n" s="2">
         <v>44795.0</v>
@@ -4800,10 +5142,13 @@
       <c r="L114" t="n">
         <v>-1.1599759139469392</v>
       </c>
+      <c r="M114" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B115" t="n">
         <v>3.0</v>
@@ -4812,13 +5157,13 @@
         <v>50776.0</v>
       </c>
       <c r="D115" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E115" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F115" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G115" t="n" s="2">
         <v>44802.0</v>
@@ -4838,10 +5183,13 @@
       <c r="L115" t="n">
         <v>-1.1073072669795128</v>
       </c>
+      <c r="M115" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B116" t="n">
         <v>3.0</v>
@@ -4850,13 +5198,13 @@
         <v>50776.0</v>
       </c>
       <c r="D116" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E116" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F116" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G116" t="n" s="2">
         <v>44826.0</v>
@@ -4876,10 +5224,13 @@
       <c r="L116" t="n">
         <v>-0.8439640321423807</v>
       </c>
+      <c r="M116" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B117" t="n">
         <v>3.0</v>
@@ -4888,13 +5239,13 @@
         <v>50776.0</v>
       </c>
       <c r="D117" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E117" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F117" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G117" t="n" s="2">
         <v>44855.0</v>
@@ -4914,10 +5265,13 @@
       <c r="L117" t="n">
         <v>-0.5542864738215355</v>
       </c>
+      <c r="M117" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B118" t="n">
         <v>3.0</v>
@@ -4926,13 +5280,13 @@
         <v>50776.0</v>
       </c>
       <c r="D118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E118" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F118" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G118" t="n" s="2">
         <v>44887.0</v>
@@ -4952,10 +5306,13 @@
       <c r="L118" t="n">
         <v>0.025068642820155095</v>
       </c>
+      <c r="M118" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B119" t="n">
         <v>3.0</v>
@@ -4964,13 +5321,13 @@
         <v>50776.0</v>
       </c>
       <c r="D119" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E119" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F119" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G119" t="n" s="2">
         <v>44908.0</v>
@@ -4990,10 +5347,13 @@
       <c r="L119" t="n">
         <v>0.3937491715921396</v>
       </c>
+      <c r="M119" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B120" t="n">
         <v>3.0</v>
@@ -5002,13 +5362,13 @@
         <v>50776.0</v>
       </c>
       <c r="D120" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E120" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F120" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G120" t="n" s="2">
         <v>44938.0</v>
@@ -5027,6 +5387,9 @@
       </c>
       <c r="L120" t="n">
         <v>0.7887640238478381</v>
+      </c>
+      <c r="M120" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>